<commit_message>
Update $UA model with latest news re. new C-Suite appointments
</commit_message>
<xml_diff>
--- a/$UA.xlsx
+++ b/$UA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6276BE66-1E95-4529-BC9B-C9DA4A97779B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C096BA0-E01B-4F0E-A722-74413E303A35}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="29835" windowHeight="18900" activeTab="1" xr2:uid="{3265DF36-E7D5-4329-9534-E494E2238873}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="29835" windowHeight="18900" xr2:uid="{3265DF36-E7D5-4329-9534-E494E2238873}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1460" uniqueCount="807">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1464" uniqueCount="810">
   <si>
     <t>$UA</t>
   </si>
@@ -2476,6 +2476,15 @@
   </si>
   <si>
     <t>Inventory/Revenue</t>
+  </si>
+  <si>
+    <t>$UA promote David Baxter to President of Americas &amp; Mehri Sehman as Chief Legal</t>
+  </si>
+  <si>
+    <t>Both are C-Suite roles. The search for a new permanent CEO continues</t>
+  </si>
+  <si>
+    <t>P/S</t>
   </si>
 </sst>
 </file>
@@ -2836,6 +2845,30 @@
       <alignment horizontal="left" indent="3"/>
     </xf>
     <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2854,12 +2887,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2870,24 +2897,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3158,7 +3167,7 @@
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>98</xdr:row>
+      <xdr:row>100</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3208,7 +3217,7 @@
     <xdr:to>
       <xdr:col>27</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>98</xdr:row>
+      <xdr:row>100</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3564,8 +3573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{749350E7-094F-4190-83AB-84EC4A5122F0}">
   <dimension ref="B2:W61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3585,41 +3594,45 @@
       </c>
     </row>
     <row r="5" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B5" s="74" t="s">
+      <c r="B5" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="75"/>
-      <c r="D5" s="76"/>
-      <c r="G5" s="74" t="s">
+      <c r="C5" s="83"/>
+      <c r="D5" s="84"/>
+      <c r="G5" s="82" t="s">
         <v>55</v>
       </c>
-      <c r="H5" s="75"/>
-      <c r="I5" s="75"/>
-      <c r="J5" s="75"/>
-      <c r="K5" s="75"/>
-      <c r="L5" s="75"/>
-      <c r="M5" s="75"/>
-      <c r="N5" s="75"/>
-      <c r="O5" s="76"/>
-      <c r="R5" s="71" t="s">
+      <c r="H5" s="83"/>
+      <c r="I5" s="83"/>
+      <c r="J5" s="83"/>
+      <c r="K5" s="83"/>
+      <c r="L5" s="83"/>
+      <c r="M5" s="83"/>
+      <c r="N5" s="83"/>
+      <c r="O5" s="84"/>
+      <c r="R5" s="79" t="s">
         <v>754</v>
       </c>
-      <c r="S5" s="72"/>
-      <c r="T5" s="72"/>
-      <c r="U5" s="72"/>
-      <c r="V5" s="72"/>
-      <c r="W5" s="73"/>
+      <c r="S5" s="80"/>
+      <c r="T5" s="80"/>
+      <c r="U5" s="80"/>
+      <c r="V5" s="80"/>
+      <c r="W5" s="81"/>
     </row>
     <row r="6" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="5">
-        <v>6.65</v>
+        <v>6.69</v>
       </c>
       <c r="D6" s="6"/>
-      <c r="G6" s="63"/>
-      <c r="H6" s="8"/>
+      <c r="G6" s="52">
+        <v>44835</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>807</v>
+      </c>
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
@@ -3660,7 +3673,9 @@
         <v>112</v>
       </c>
       <c r="G7" s="63"/>
-      <c r="H7" s="8"/>
+      <c r="H7" s="61" t="s">
+        <v>808</v>
+      </c>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
       <c r="K7" s="8"/>
@@ -3697,7 +3712,7 @@
       </c>
       <c r="C8" s="28">
         <f>C6*C7</f>
-        <v>3048.36</v>
+        <v>3066.6959999999999</v>
       </c>
       <c r="D8" s="30"/>
       <c r="G8" s="63"/>
@@ -3871,7 +3886,7 @@
       </c>
       <c r="C12" s="29">
         <f>C8-C11</f>
-        <v>2671.7809999999999</v>
+        <v>2690.1169999999997</v>
       </c>
       <c r="D12" s="31"/>
       <c r="G12" s="63"/>
@@ -3979,11 +3994,11 @@
       </c>
     </row>
     <row r="15" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B15" s="74" t="s">
+      <c r="B15" s="82" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="75"/>
-      <c r="D15" s="76"/>
+      <c r="C15" s="83"/>
+      <c r="D15" s="84"/>
       <c r="G15" s="63"/>
       <c r="H15" s="8"/>
       <c r="I15" s="8"/>
@@ -4020,10 +4035,10 @@
       <c r="B16" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="77" t="s">
+      <c r="C16" s="75" t="s">
         <v>63</v>
       </c>
-      <c r="D16" s="78"/>
+      <c r="D16" s="76"/>
       <c r="G16" s="52">
         <v>44682</v>
       </c>
@@ -4064,10 +4079,10 @@
       <c r="B17" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="77" t="s">
+      <c r="C17" s="75" t="s">
         <v>64</v>
       </c>
-      <c r="D17" s="78"/>
+      <c r="D17" s="76"/>
       <c r="G17" s="63"/>
       <c r="H17" s="61" t="s">
         <v>774</v>
@@ -4106,10 +4121,10 @@
       <c r="B18" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="C18" s="77" t="s">
+      <c r="C18" s="75" t="s">
         <v>65</v>
       </c>
-      <c r="D18" s="78"/>
+      <c r="D18" s="76"/>
       <c r="G18" s="63"/>
       <c r="H18" s="8"/>
       <c r="I18" s="8"/>
@@ -4146,10 +4161,10 @@
       <c r="B19" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="C19" s="79" t="s">
+      <c r="C19" s="85" t="s">
         <v>67</v>
       </c>
-      <c r="D19" s="80"/>
+      <c r="D19" s="86"/>
       <c r="E19" s="1" t="s">
         <v>773</v>
       </c>
@@ -4258,11 +4273,11 @@
       </c>
     </row>
     <row r="22" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B22" s="74" t="s">
+      <c r="B22" s="82" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="75"/>
-      <c r="D22" s="76"/>
+      <c r="C22" s="83"/>
+      <c r="D22" s="84"/>
       <c r="G22" s="14" t="s">
         <v>31</v>
       </c>
@@ -4303,10 +4318,10 @@
       <c r="B23" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="77" t="s">
+      <c r="C23" s="75" t="s">
         <v>59</v>
       </c>
-      <c r="D23" s="78"/>
+      <c r="D23" s="76"/>
       <c r="G23" s="63"/>
       <c r="H23" s="8"/>
       <c r="I23" s="8"/>
@@ -4343,10 +4358,10 @@
       <c r="B24" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="77">
+      <c r="C24" s="75">
         <v>1996</v>
       </c>
-      <c r="D24" s="78"/>
+      <c r="D24" s="76"/>
       <c r="G24" s="52">
         <v>44228</v>
       </c>
@@ -4425,10 +4440,10 @@
       <c r="B26" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="C26" s="77">
+      <c r="C26" s="75">
         <v>422</v>
       </c>
-      <c r="D26" s="78"/>
+      <c r="D26" s="76"/>
       <c r="G26" s="64"/>
       <c r="H26" s="10"/>
       <c r="I26" s="10"/>
@@ -4465,11 +4480,11 @@
       <c r="B27" s="14" t="s">
         <v>779</v>
       </c>
-      <c r="C27" s="81">
+      <c r="C27" s="87">
         <f>'Financial Model'!Q52</f>
         <v>954.39400000000001</v>
       </c>
-      <c r="D27" s="82"/>
+      <c r="D27" s="88"/>
       <c r="R27" s="37">
         <v>2020</v>
       </c>
@@ -4524,10 +4539,10 @@
       <c r="B29" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C29" s="77" t="s">
+      <c r="C29" s="75" t="s">
         <v>789</v>
       </c>
-      <c r="D29" s="78"/>
+      <c r="D29" s="76"/>
       <c r="R29" s="37">
         <v>2020</v>
       </c>
@@ -4555,10 +4570,10 @@
       <c r="B30" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C30" s="87" t="s">
+      <c r="C30" s="77" t="s">
         <v>18</v>
       </c>
-      <c r="D30" s="88"/>
+      <c r="D30" s="78"/>
       <c r="R30" s="37">
         <v>2020</v>
       </c>
@@ -4631,11 +4646,11 @@
       </c>
     </row>
     <row r="33" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B33" s="74" t="s">
+      <c r="B33" s="82" t="s">
         <v>56</v>
       </c>
-      <c r="C33" s="75"/>
-      <c r="D33" s="76"/>
+      <c r="C33" s="83"/>
+      <c r="D33" s="84"/>
       <c r="R33" s="37">
         <v>2020</v>
       </c>
@@ -4663,11 +4678,11 @@
       <c r="B34" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C34" s="85">
+      <c r="C34" s="73">
         <f>C12/SUM('Financial Model'!N20:Q20)</f>
-        <v>15.608659075905694</v>
-      </c>
-      <c r="D34" s="86"/>
+        <v>15.715778773521555</v>
+      </c>
+      <c r="D34" s="74"/>
       <c r="R34" s="37">
         <v>2020</v>
       </c>
@@ -4695,11 +4710,11 @@
       <c r="B35" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="C35" s="85">
+      <c r="C35" s="73">
         <f>C6/SUM('Financial Model'!N21:Q21)</f>
-        <v>18.371878693929585</v>
-      </c>
-      <c r="D35" s="86"/>
+        <v>18.4823862349457</v>
+      </c>
+      <c r="D35" s="74"/>
       <c r="R35" s="37">
         <v>2020</v>
       </c>
@@ -4727,8 +4742,8 @@
       <c r="B36" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="C36" s="77"/>
-      <c r="D36" s="78"/>
+      <c r="C36" s="75"/>
+      <c r="D36" s="76"/>
       <c r="R36" s="37">
         <v>2020</v>
       </c>
@@ -4756,11 +4771,11 @@
       <c r="B37" s="14" t="s">
         <v>778</v>
       </c>
-      <c r="C37" s="85">
+      <c r="C37" s="73">
         <f>C6/'Financial Model'!Q77</f>
-        <v>1.7630377451788364</v>
-      </c>
-      <c r="D37" s="86"/>
+        <v>1.7736424834957014</v>
+      </c>
+      <c r="D37" s="74"/>
       <c r="R37" s="37">
         <v>2020</v>
       </c>
@@ -4869,11 +4884,11 @@
       <c r="B41" s="15" t="s">
         <v>775</v>
       </c>
-      <c r="C41" s="83">
+      <c r="C41" s="71">
         <f>C6/'Financial Model'!AA21</f>
-        <v>8.5974604232627811</v>
-      </c>
-      <c r="D41" s="84"/>
+        <v>8.6491744709215048</v>
+      </c>
+      <c r="D41" s="72"/>
       <c r="R41" s="37">
         <v>2019</v>
       </c>
@@ -5363,16 +5378,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C29:D29"/>
     <mergeCell ref="R5:W5"/>
     <mergeCell ref="G5:O5"/>
     <mergeCell ref="B33:D33"/>
@@ -5384,6 +5389,16 @@
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C29:D29"/>
   </mergeCells>
   <conditionalFormatting sqref="V8:V24">
     <cfRule type="cellIs" dxfId="33" priority="37" operator="greaterThan">
@@ -5532,13 +5547,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E32081CA-472C-4CAE-89FB-0831C607DA60}">
-  <dimension ref="B1:AT92"/>
+  <dimension ref="B1:AT94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C66" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="P5" sqref="P5"/>
+      <selection pane="bottomRight" activeCell="M94" sqref="M94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7639,6 +7654,10 @@
         <f>Q60-Q71</f>
         <v>1729.0950000000003</v>
       </c>
+      <c r="AA76" s="22">
+        <f>AA60-AA71</f>
+        <v>2088.9940000000006</v>
+      </c>
     </row>
     <row r="77" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B77" s="1" t="s">
@@ -7652,6 +7671,10 @@
         <f>Q76/Q22</f>
         <v>3.7718988253002195</v>
       </c>
+      <c r="AA77" s="53">
+        <f>AA76/AA22</f>
+        <v>4.4875962397745255</v>
+      </c>
     </row>
     <row r="79" spans="2:27" s="58" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B79" s="58" t="s">
@@ -7812,34 +7835,56 @@
     </row>
     <row r="90" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B90" s="1" t="s">
+        <v>778</v>
+      </c>
+      <c r="P90" s="70">
+        <f t="shared" ref="P90:Q90" si="25">P86/P77</f>
+        <v>4.3844509454849581</v>
+      </c>
+      <c r="Q90" s="70">
+        <f>Q86/Q77</f>
+        <v>2.0095979110459519</v>
+      </c>
+      <c r="AA90" s="70">
+        <f>AA86/AA77</f>
+        <v>4.0199694972795506</v>
+      </c>
+    </row>
+    <row r="91" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B91" s="1" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="92" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B92" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="Y90" s="70">
-        <f t="shared" ref="Y90:Z90" si="25">Y86/Y21</f>
+      <c r="Y92" s="70">
+        <f t="shared" ref="Y92:Z92" si="26">Y86/Y21</f>
         <v>93.871302120640664</v>
       </c>
-      <c r="Z90" s="70">
-        <f t="shared" si="25"/>
+      <c r="Z92" s="70">
+        <f t="shared" si="26"/>
         <v>-12.303582123796154</v>
       </c>
-      <c r="AA90" s="70">
+      <c r="AA92" s="70">
         <f>AA86/AA21</f>
         <v>23.323035494084294</v>
       </c>
     </row>
-    <row r="92" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B92" s="1" t="s">
+    <row r="94" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B94" s="1" t="s">
         <v>806</v>
       </c>
-      <c r="P92" s="25">
-        <f t="shared" ref="P92:Q92" si="26">P52/P9</f>
+      <c r="P94" s="25">
+        <f t="shared" ref="P94" si="27">P52/P9</f>
         <v>0.63373547690332799</v>
       </c>
-      <c r="Q92" s="25">
+      <c r="Q94" s="25">
         <f>Q52/Q9</f>
         <v>0.70745268732158828</v>
       </c>
-      <c r="AA92" s="25">
+      <c r="AA94" s="25">
         <f>AA52/AA9</f>
         <v>0.14276675535667846</v>
       </c>

</xml_diff>

<commit_message>
More backdated metric calcs to $UA, update Fashion Retailers overview sheet
</commit_message>
<xml_diff>
--- a/$UA.xlsx
+++ b/$UA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Stocks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEADE0F0-A2FD-C640-8D86-07B98865F0D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F71C4383-8C71-8543-9E7D-A7AA9EF4B7DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="29840" windowHeight="18900" activeTab="1" xr2:uid="{3265DF36-E7D5-4329-9534-E494E2238873}"/>
   </bookViews>
@@ -2849,30 +2849,7 @@
       <alignment horizontal="left" indent="3"/>
     </xf>
     <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="1" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2891,6 +2868,12 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2903,7 +2886,24 @@
     <xf numFmtId="166" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="168" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3605,30 +3605,30 @@
       </c>
     </row>
     <row r="5" spans="2:23" x14ac:dyDescent="0.15">
-      <c r="B5" s="82" t="s">
+      <c r="B5" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="83"/>
-      <c r="D5" s="84"/>
-      <c r="G5" s="82" t="s">
+      <c r="C5" s="76"/>
+      <c r="D5" s="77"/>
+      <c r="G5" s="75" t="s">
         <v>55</v>
       </c>
-      <c r="H5" s="83"/>
-      <c r="I5" s="83"/>
-      <c r="J5" s="83"/>
-      <c r="K5" s="83"/>
-      <c r="L5" s="83"/>
-      <c r="M5" s="83"/>
-      <c r="N5" s="83"/>
-      <c r="O5" s="84"/>
-      <c r="R5" s="79" t="s">
+      <c r="H5" s="76"/>
+      <c r="I5" s="76"/>
+      <c r="J5" s="76"/>
+      <c r="K5" s="76"/>
+      <c r="L5" s="76"/>
+      <c r="M5" s="76"/>
+      <c r="N5" s="76"/>
+      <c r="O5" s="77"/>
+      <c r="R5" s="72" t="s">
         <v>754</v>
       </c>
-      <c r="S5" s="80"/>
-      <c r="T5" s="80"/>
-      <c r="U5" s="80"/>
-      <c r="V5" s="80"/>
-      <c r="W5" s="81"/>
+      <c r="S5" s="73"/>
+      <c r="T5" s="73"/>
+      <c r="U5" s="73"/>
+      <c r="V5" s="73"/>
+      <c r="W5" s="74"/>
     </row>
     <row r="6" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B6" s="4" t="s">
@@ -4005,11 +4005,11 @@
       </c>
     </row>
     <row r="15" spans="2:23" x14ac:dyDescent="0.15">
-      <c r="B15" s="82" t="s">
+      <c r="B15" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="83"/>
-      <c r="D15" s="84"/>
+      <c r="C15" s="76"/>
+      <c r="D15" s="77"/>
       <c r="G15" s="63"/>
       <c r="H15" s="8"/>
       <c r="I15" s="8"/>
@@ -4046,10 +4046,10 @@
       <c r="B16" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="75" t="s">
+      <c r="C16" s="78" t="s">
         <v>63</v>
       </c>
-      <c r="D16" s="76"/>
+      <c r="D16" s="79"/>
       <c r="G16" s="52">
         <v>44682</v>
       </c>
@@ -4090,10 +4090,10 @@
       <c r="B17" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="75" t="s">
+      <c r="C17" s="78" t="s">
         <v>64</v>
       </c>
-      <c r="D17" s="76"/>
+      <c r="D17" s="79"/>
       <c r="G17" s="63"/>
       <c r="H17" s="61" t="s">
         <v>774</v>
@@ -4132,10 +4132,10 @@
       <c r="B18" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="C18" s="75" t="s">
+      <c r="C18" s="78" t="s">
         <v>65</v>
       </c>
-      <c r="D18" s="76"/>
+      <c r="D18" s="79"/>
       <c r="G18" s="63"/>
       <c r="H18" s="8"/>
       <c r="I18" s="8"/>
@@ -4172,10 +4172,10 @@
       <c r="B19" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="C19" s="85" t="s">
+      <c r="C19" s="80" t="s">
         <v>67</v>
       </c>
-      <c r="D19" s="86"/>
+      <c r="D19" s="81"/>
       <c r="E19" s="1" t="s">
         <v>773</v>
       </c>
@@ -4284,11 +4284,11 @@
       </c>
     </row>
     <row r="22" spans="2:23" x14ac:dyDescent="0.15">
-      <c r="B22" s="82" t="s">
+      <c r="B22" s="75" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="83"/>
-      <c r="D22" s="84"/>
+      <c r="C22" s="76"/>
+      <c r="D22" s="77"/>
       <c r="G22" s="14" t="s">
         <v>31</v>
       </c>
@@ -4329,10 +4329,10 @@
       <c r="B23" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="75" t="s">
+      <c r="C23" s="78" t="s">
         <v>59</v>
       </c>
-      <c r="D23" s="76"/>
+      <c r="D23" s="79"/>
       <c r="G23" s="63"/>
       <c r="H23" s="8"/>
       <c r="I23" s="8"/>
@@ -4369,10 +4369,10 @@
       <c r="B24" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="75">
+      <c r="C24" s="78">
         <v>1996</v>
       </c>
-      <c r="D24" s="76"/>
+      <c r="D24" s="79"/>
       <c r="G24" s="52">
         <v>44228</v>
       </c>
@@ -4451,10 +4451,10 @@
       <c r="B26" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="C26" s="75">
+      <c r="C26" s="78">
         <v>422</v>
       </c>
-      <c r="D26" s="76"/>
+      <c r="D26" s="79"/>
       <c r="G26" s="64"/>
       <c r="H26" s="10"/>
       <c r="I26" s="10"/>
@@ -4491,11 +4491,11 @@
       <c r="B27" s="14" t="s">
         <v>779</v>
       </c>
-      <c r="C27" s="87">
+      <c r="C27" s="82">
         <f>'Financial Model'!Q52</f>
         <v>954.39400000000001</v>
       </c>
-      <c r="D27" s="88"/>
+      <c r="D27" s="83"/>
       <c r="R27" s="37">
         <v>2020</v>
       </c>
@@ -4550,10 +4550,10 @@
       <c r="B29" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C29" s="75" t="s">
+      <c r="C29" s="78" t="s">
         <v>789</v>
       </c>
-      <c r="D29" s="76"/>
+      <c r="D29" s="79"/>
       <c r="R29" s="37">
         <v>2020</v>
       </c>
@@ -4581,10 +4581,10 @@
       <c r="B30" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C30" s="77" t="s">
+      <c r="C30" s="88" t="s">
         <v>18</v>
       </c>
-      <c r="D30" s="78"/>
+      <c r="D30" s="89"/>
       <c r="R30" s="37">
         <v>2020</v>
       </c>
@@ -4657,11 +4657,11 @@
       </c>
     </row>
     <row r="33" spans="2:23" x14ac:dyDescent="0.15">
-      <c r="B33" s="82" t="s">
+      <c r="B33" s="75" t="s">
         <v>56</v>
       </c>
-      <c r="C33" s="83"/>
-      <c r="D33" s="84"/>
+      <c r="C33" s="76"/>
+      <c r="D33" s="77"/>
       <c r="R33" s="37">
         <v>2020</v>
       </c>
@@ -4689,11 +4689,11 @@
       <c r="B34" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C34" s="73">
+      <c r="C34" s="86">
         <f>C12/SUM('Financial Model'!N20:Q20)</f>
         <v>15.715778773521555</v>
       </c>
-      <c r="D34" s="74"/>
+      <c r="D34" s="87"/>
       <c r="R34" s="37">
         <v>2020</v>
       </c>
@@ -4721,11 +4721,11 @@
       <c r="B35" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="C35" s="73">
+      <c r="C35" s="86">
         <f>C6/SUM('Financial Model'!N21:Q21)</f>
         <v>18.4823862349457</v>
       </c>
-      <c r="D35" s="74"/>
+      <c r="D35" s="87"/>
       <c r="R35" s="37">
         <v>2020</v>
       </c>
@@ -4753,8 +4753,8 @@
       <c r="B36" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="C36" s="75"/>
-      <c r="D36" s="76"/>
+      <c r="C36" s="78"/>
+      <c r="D36" s="79"/>
       <c r="R36" s="37">
         <v>2020</v>
       </c>
@@ -4782,11 +4782,11 @@
       <c r="B37" s="14" t="s">
         <v>778</v>
       </c>
-      <c r="C37" s="73">
+      <c r="C37" s="86">
         <f>C6/'Financial Model'!Q77</f>
         <v>1.7736424834957014</v>
       </c>
-      <c r="D37" s="74"/>
+      <c r="D37" s="87"/>
       <c r="R37" s="37">
         <v>2020</v>
       </c>
@@ -4905,11 +4905,11 @@
       <c r="B41" s="15" t="s">
         <v>775</v>
       </c>
-      <c r="C41" s="71">
+      <c r="C41" s="84">
         <f>C6/'Financial Model'!AA21</f>
         <v>8.6491744709215048</v>
       </c>
-      <c r="D41" s="72"/>
+      <c r="D41" s="85"/>
       <c r="R41" s="37">
         <v>2019</v>
       </c>
@@ -5399,17 +5399,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="R5:W5"/>
-    <mergeCell ref="G5:O5"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C27:D27"/>
     <mergeCell ref="C41:D41"/>
     <mergeCell ref="C34:D34"/>
     <mergeCell ref="C35:D35"/>
@@ -5422,6 +5411,17 @@
     <mergeCell ref="C29:D29"/>
     <mergeCell ref="C38:D38"/>
     <mergeCell ref="C39:D39"/>
+    <mergeCell ref="R5:W5"/>
+    <mergeCell ref="G5:O5"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C27:D27"/>
   </mergeCells>
   <conditionalFormatting sqref="V8:V24">
     <cfRule type="cellIs" dxfId="33" priority="37" operator="greaterThan">
@@ -5576,10 +5576,10 @@
   <dimension ref="B1:AT95"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C27" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="H43" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="K43" sqref="K43"/>
+      <selection pane="bottomRight" activeCell="AA79" sqref="AA79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -7984,7 +7984,7 @@
         <v>1675.9930000000004</v>
       </c>
       <c r="O76" s="22">
-        <f t="shared" ref="O76:P76" si="24">O60-O71</f>
+        <f t="shared" ref="O76" si="24">O60-O71</f>
         <v>2088.9740000000011</v>
       </c>
       <c r="P76" s="22">
@@ -8037,8 +8037,12 @@
       <c r="B79" s="58" t="s">
         <v>790</v>
       </c>
-      <c r="O79" s="89">
+      <c r="O79" s="71">
         <f>O52/K52-1</f>
+        <v>-9.4382203054999447E-2</v>
+      </c>
+      <c r="AA79" s="71">
+        <f>AA52/Z52-1</f>
         <v>-9.4382203054999447E-2</v>
       </c>
     </row>
@@ -8047,7 +8051,7 @@
         <v>791</v>
       </c>
       <c r="P80" s="66">
-        <f t="shared" ref="P80:Q80" si="28">P52/O52-1</f>
+        <f t="shared" ref="P80" si="28">P52/O52-1</f>
         <v>1.6076952465461369E-2</v>
       </c>
       <c r="Q80" s="66">
@@ -8294,7 +8298,7 @@
         <v>2.0095979110459519</v>
       </c>
       <c r="Z90" s="70">
-        <f t="shared" ref="Z90:AA90" si="45">Z86/Z77</f>
+        <f t="shared" ref="Z90" si="45">Z86/Z77</f>
         <v>4.0379570081736604</v>
       </c>
       <c r="AA90" s="70">
@@ -8335,7 +8339,7 @@
         <v>0.6221570503604078</v>
       </c>
       <c r="Z91" s="70">
-        <f t="shared" ref="Z91:AA91" si="47">Z87/Z6</f>
+        <f t="shared" ref="Z91" si="47">Z87/Z6</f>
         <v>1.5969938669011909</v>
       </c>
       <c r="AA91" s="70">
@@ -8393,7 +8397,7 @@
         <v>810</v>
       </c>
       <c r="Z93" s="70">
-        <f t="shared" ref="Z93:AA93" si="54">Z88/Z6</f>
+        <f t="shared" ref="Z93" si="54">Z88/Z6</f>
         <v>1.4755550124711148</v>
       </c>
       <c r="AA93" s="70">
@@ -8414,7 +8418,7 @@
         <v>0.63826449707429866</v>
       </c>
       <c r="O95" s="25">
-        <f t="shared" ref="N95:P95" si="56">O52/O9</f>
+        <f t="shared" ref="O95:P95" si="56">O52/O9</f>
         <v>0.53060904195317171</v>
       </c>
       <c r="P95" s="25">
@@ -8426,7 +8430,7 @@
         <v>0.70745268732158828</v>
       </c>
       <c r="Z95" s="25">
-        <f t="shared" ref="Z95:AA95" si="57">Z52/Z9</f>
+        <f t="shared" ref="Z95" si="57">Z52/Z9</f>
         <v>0.20023255361795636</v>
       </c>
       <c r="AA95" s="25">

</xml_diff>

<commit_message>
Add Q321, Q320 financial data
</commit_message>
<xml_diff>
--- a/$UA.xlsx
+++ b/$UA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{953A6228-E65D-4ACE-97AB-76ADEF5E8911}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9065FAFC-8C88-4D00-87A6-74436F4D858F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="29835" windowHeight="18900" activeTab="1" xr2:uid="{3265DF36-E7D5-4329-9534-E494E2238873}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="29835" windowHeight="18900" xr2:uid="{3265DF36-E7D5-4329-9534-E494E2238873}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -2998,6 +2998,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="10" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="1" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3058,7 +3059,6 @@
     <xf numFmtId="166" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3733,8 +3733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{749350E7-094F-4190-83AB-84EC4A5122F0}">
   <dimension ref="B2:W61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C35" sqref="C35:D35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3754,37 +3754,37 @@
       </c>
     </row>
     <row r="5" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B5" s="114" t="s">
+      <c r="B5" s="115" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="115"/>
-      <c r="D5" s="116"/>
-      <c r="G5" s="114" t="s">
+      <c r="C5" s="116"/>
+      <c r="D5" s="117"/>
+      <c r="G5" s="115" t="s">
         <v>55</v>
       </c>
-      <c r="H5" s="115"/>
-      <c r="I5" s="115"/>
-      <c r="J5" s="115"/>
-      <c r="K5" s="115"/>
-      <c r="L5" s="115"/>
-      <c r="M5" s="115"/>
-      <c r="N5" s="115"/>
-      <c r="O5" s="116"/>
-      <c r="R5" s="111" t="s">
+      <c r="H5" s="116"/>
+      <c r="I5" s="116"/>
+      <c r="J5" s="116"/>
+      <c r="K5" s="116"/>
+      <c r="L5" s="116"/>
+      <c r="M5" s="116"/>
+      <c r="N5" s="116"/>
+      <c r="O5" s="117"/>
+      <c r="R5" s="112" t="s">
         <v>754</v>
       </c>
-      <c r="S5" s="112"/>
-      <c r="T5" s="112"/>
-      <c r="U5" s="112"/>
-      <c r="V5" s="112"/>
-      <c r="W5" s="113"/>
+      <c r="S5" s="113"/>
+      <c r="T5" s="113"/>
+      <c r="U5" s="113"/>
+      <c r="V5" s="113"/>
+      <c r="W5" s="114"/>
     </row>
     <row r="6" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="5">
-        <v>6.69</v>
+        <v>6.48</v>
       </c>
       <c r="D6" s="6"/>
       <c r="G6" s="52">
@@ -3872,7 +3872,7 @@
       </c>
       <c r="C8" s="28">
         <f>C6*C7</f>
-        <v>3066.6959999999999</v>
+        <v>2970.4320000000002</v>
       </c>
       <c r="D8" s="30"/>
       <c r="G8" s="63"/>
@@ -4046,7 +4046,7 @@
       </c>
       <c r="C12" s="29">
         <f>C8-C11</f>
-        <v>2690.1169999999997</v>
+        <v>2593.8530000000001</v>
       </c>
       <c r="D12" s="31"/>
       <c r="G12" s="63"/>
@@ -4154,11 +4154,11 @@
       </c>
     </row>
     <row r="15" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B15" s="114" t="s">
+      <c r="B15" s="115" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="115"/>
-      <c r="D15" s="116"/>
+      <c r="C15" s="116"/>
+      <c r="D15" s="117"/>
       <c r="G15" s="63"/>
       <c r="H15" s="8"/>
       <c r="I15" s="8"/>
@@ -4195,10 +4195,10 @@
       <c r="B16" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="105" t="s">
+      <c r="C16" s="106" t="s">
         <v>63</v>
       </c>
-      <c r="D16" s="106"/>
+      <c r="D16" s="107"/>
       <c r="G16" s="52">
         <v>44682</v>
       </c>
@@ -4239,10 +4239,10 @@
       <c r="B17" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="105" t="s">
+      <c r="C17" s="106" t="s">
         <v>64</v>
       </c>
-      <c r="D17" s="106"/>
+      <c r="D17" s="107"/>
       <c r="G17" s="63"/>
       <c r="H17" s="61" t="s">
         <v>774</v>
@@ -4281,10 +4281,10 @@
       <c r="B18" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="C18" s="105" t="s">
+      <c r="C18" s="106" t="s">
         <v>65</v>
       </c>
-      <c r="D18" s="106"/>
+      <c r="D18" s="107"/>
       <c r="G18" s="63"/>
       <c r="H18" s="8"/>
       <c r="I18" s="8"/>
@@ -4321,10 +4321,10 @@
       <c r="B19" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="C19" s="117" t="s">
+      <c r="C19" s="118" t="s">
         <v>67</v>
       </c>
-      <c r="D19" s="118"/>
+      <c r="D19" s="119"/>
       <c r="E19" s="1" t="s">
         <v>773</v>
       </c>
@@ -4433,11 +4433,11 @@
       </c>
     </row>
     <row r="22" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B22" s="114" t="s">
+      <c r="B22" s="115" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="115"/>
-      <c r="D22" s="116"/>
+      <c r="C22" s="116"/>
+      <c r="D22" s="117"/>
       <c r="G22" s="14" t="s">
         <v>31</v>
       </c>
@@ -4478,10 +4478,10 @@
       <c r="B23" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="105" t="s">
+      <c r="C23" s="106" t="s">
         <v>59</v>
       </c>
-      <c r="D23" s="106"/>
+      <c r="D23" s="107"/>
       <c r="G23" s="63"/>
       <c r="H23" s="8"/>
       <c r="I23" s="8"/>
@@ -4518,10 +4518,10 @@
       <c r="B24" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="105">
+      <c r="C24" s="106">
         <v>1996</v>
       </c>
-      <c r="D24" s="106"/>
+      <c r="D24" s="107"/>
       <c r="G24" s="52">
         <v>44228</v>
       </c>
@@ -4600,10 +4600,10 @@
       <c r="B26" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="C26" s="105">
+      <c r="C26" s="106">
         <v>422</v>
       </c>
-      <c r="D26" s="106"/>
+      <c r="D26" s="107"/>
       <c r="G26" s="64"/>
       <c r="H26" s="10"/>
       <c r="I26" s="10"/>
@@ -4640,11 +4640,11 @@
       <c r="B27" s="14" t="s">
         <v>779</v>
       </c>
-      <c r="C27" s="119">
+      <c r="C27" s="120">
         <f>'Financial Model'!Q52</f>
         <v>954.39400000000001</v>
       </c>
-      <c r="D27" s="120"/>
+      <c r="D27" s="121"/>
       <c r="R27" s="37">
         <v>2020</v>
       </c>
@@ -4699,10 +4699,10 @@
       <c r="B29" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C29" s="105" t="s">
+      <c r="C29" s="106" t="s">
         <v>789</v>
       </c>
-      <c r="D29" s="106"/>
+      <c r="D29" s="107"/>
       <c r="R29" s="37">
         <v>2020</v>
       </c>
@@ -4730,10 +4730,10 @@
       <c r="B30" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C30" s="107" t="s">
+      <c r="C30" s="108" t="s">
         <v>18</v>
       </c>
-      <c r="D30" s="108"/>
+      <c r="D30" s="109"/>
       <c r="R30" s="37">
         <v>2020</v>
       </c>
@@ -4806,11 +4806,11 @@
       </c>
     </row>
     <row r="33" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B33" s="114" t="s">
+      <c r="B33" s="115" t="s">
         <v>56</v>
       </c>
-      <c r="C33" s="115"/>
-      <c r="D33" s="116"/>
+      <c r="C33" s="116"/>
+      <c r="D33" s="117"/>
       <c r="R33" s="37">
         <v>2020</v>
       </c>
@@ -4838,11 +4838,11 @@
       <c r="B34" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C34" s="103">
+      <c r="C34" s="104">
         <f>C12/SUM('Financial Model'!N20:Q20)</f>
-        <v>15.715778773521555</v>
-      </c>
-      <c r="D34" s="104"/>
+        <v>15.153400361038278</v>
+      </c>
+      <c r="D34" s="105"/>
       <c r="R34" s="37">
         <v>2020</v>
       </c>
@@ -4870,11 +4870,11 @@
       <c r="B35" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="C35" s="103">
+      <c r="C35" s="104">
         <f>C6/SUM('Financial Model'!N21:Q21)</f>
-        <v>18.4823862349457</v>
-      </c>
-      <c r="D35" s="104"/>
+        <v>17.902221644611082</v>
+      </c>
+      <c r="D35" s="105"/>
       <c r="R35" s="37">
         <v>2020</v>
       </c>
@@ -4902,8 +4902,8 @@
       <c r="B36" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="C36" s="105"/>
-      <c r="D36" s="106"/>
+      <c r="C36" s="106"/>
+      <c r="D36" s="107"/>
       <c r="R36" s="37">
         <v>2020</v>
       </c>
@@ -4931,11 +4931,11 @@
       <c r="B37" s="14" t="s">
         <v>778</v>
       </c>
-      <c r="C37" s="103">
+      <c r="C37" s="104">
         <f>C6/'Financial Model'!Q77</f>
-        <v>1.7736424834957014</v>
-      </c>
-      <c r="D37" s="104"/>
+        <v>1.7179676073321593</v>
+      </c>
+      <c r="D37" s="105"/>
       <c r="R37" s="37">
         <v>2020</v>
       </c>
@@ -4963,11 +4963,11 @@
       <c r="B38" s="14" t="s">
         <v>809</v>
       </c>
-      <c r="C38" s="109">
+      <c r="C38" s="110">
         <f>C8/SUM('Financial Model'!N9:Q9)</f>
-        <v>0.53569184551470383</v>
-      </c>
-      <c r="D38" s="110"/>
+        <v>0.51887640641782984</v>
+      </c>
+      <c r="D38" s="111"/>
       <c r="R38" s="37">
         <v>2019</v>
       </c>
@@ -4995,11 +4995,11 @@
       <c r="B39" s="14" t="s">
         <v>810</v>
       </c>
-      <c r="C39" s="109">
+      <c r="C39" s="110">
         <f>C12/SUM('Financial Model'!N9:Q9)</f>
-        <v>0.46991085532458332</v>
-      </c>
-      <c r="D39" s="110"/>
+        <v>0.45309541622770927</v>
+      </c>
+      <c r="D39" s="111"/>
       <c r="R39" s="37">
         <v>2019</v>
       </c>
@@ -5054,11 +5054,11 @@
       <c r="B41" s="15" t="s">
         <v>775</v>
       </c>
-      <c r="C41" s="101">
+      <c r="C41" s="102">
         <f>C6/'Financial Model'!AA21</f>
-        <v>8.6491744709215048</v>
-      </c>
-      <c r="D41" s="102"/>
+        <v>8.3776757207132064</v>
+      </c>
+      <c r="D41" s="103"/>
       <c r="R41" s="37">
         <v>2019</v>
       </c>
@@ -5724,11 +5724,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E32081CA-472C-4CAE-89FB-0831C607DA60}">
   <dimension ref="B1:BR107"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I31" sqref="I29:P31"/>
+      <selection pane="bottomRight" activeCell="L92" sqref="L92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7852,131 +7852,131 @@
       </c>
       <c r="AM20" s="55">
         <f>AL20*(1+$AO$24)</f>
-        <v>1289.4645001550518</v>
+        <v>1263.930549656932</v>
       </c>
       <c r="AN20" s="55">
         <f t="shared" ref="AN20:BR20" si="34">AM20*(1+$AO$24)</f>
-        <v>1302.3591451566024</v>
+        <v>1251.2912441603628</v>
       </c>
       <c r="AO20" s="55">
         <f t="shared" si="34"/>
-        <v>1315.3827366081684</v>
+        <v>1238.7783317187591</v>
       </c>
       <c r="AP20" s="55">
         <f t="shared" si="34"/>
-        <v>1328.5365639742502</v>
+        <v>1226.3905484015716</v>
       </c>
       <c r="AQ20" s="55">
         <f t="shared" si="34"/>
-        <v>1341.8219296139928</v>
+        <v>1214.1266429175557</v>
       </c>
       <c r="AR20" s="55">
         <f t="shared" si="34"/>
-        <v>1355.2401489101328</v>
+        <v>1201.9853764883801</v>
       </c>
       <c r="AS20" s="55">
         <f t="shared" si="34"/>
-        <v>1368.7925503992342</v>
+        <v>1189.9655227234962</v>
       </c>
       <c r="AT20" s="55">
         <f t="shared" si="34"/>
-        <v>1382.4804759032265</v>
+        <v>1178.0658674962613</v>
       </c>
       <c r="AU20" s="55">
         <f t="shared" si="34"/>
-        <v>1396.3052806622588</v>
+        <v>1166.2852088212987</v>
       </c>
       <c r="AV20" s="55">
         <f t="shared" si="34"/>
-        <v>1410.2683334688813</v>
+        <v>1154.6223567330858</v>
       </c>
       <c r="AW20" s="55">
         <f t="shared" si="34"/>
-        <v>1424.3710168035702</v>
+        <v>1143.076133165755</v>
       </c>
       <c r="AX20" s="55">
         <f t="shared" si="34"/>
-        <v>1438.6147269716059</v>
+        <v>1131.6453718340974</v>
       </c>
       <c r="AY20" s="55">
         <f t="shared" si="34"/>
-        <v>1453.000874241322</v>
+        <v>1120.3289181157566</v>
       </c>
       <c r="AZ20" s="55">
         <f t="shared" si="34"/>
-        <v>1467.5308829837352</v>
+        <v>1109.125628934599</v>
       </c>
       <c r="BA20" s="55">
         <f t="shared" si="34"/>
-        <v>1482.2061918135726</v>
+        <v>1098.0343726452531</v>
       </c>
       <c r="BB20" s="55">
         <f t="shared" si="34"/>
-        <v>1497.0282537317082</v>
+        <v>1087.0540289188007</v>
       </c>
       <c r="BC20" s="55">
         <f t="shared" si="34"/>
-        <v>1511.9985362690254</v>
+        <v>1076.1834886296126</v>
       </c>
       <c r="BD20" s="55">
         <f t="shared" si="34"/>
-        <v>1527.1185216317156</v>
+        <v>1065.4216537433165</v>
       </c>
       <c r="BE20" s="55">
         <f t="shared" si="34"/>
-        <v>1542.3897068480328</v>
+        <v>1054.7674372058832</v>
       </c>
       <c r="BF20" s="55">
         <f t="shared" si="34"/>
-        <v>1557.8136039165131</v>
+        <v>1044.2197628338245</v>
       </c>
       <c r="BG20" s="55">
         <f t="shared" si="34"/>
-        <v>1573.3917399556783</v>
+        <v>1033.7775652054861</v>
       </c>
       <c r="BH20" s="55">
         <f t="shared" si="34"/>
-        <v>1589.125657355235</v>
+        <v>1023.4397895534312</v>
       </c>
       <c r="BI20" s="55">
         <f t="shared" si="34"/>
-        <v>1605.0169139287873</v>
+        <v>1013.2053916578968</v>
       </c>
       <c r="BJ20" s="55">
         <f t="shared" si="34"/>
-        <v>1621.0670830680751</v>
+        <v>1003.0733377413178</v>
       </c>
       <c r="BK20" s="55">
         <f t="shared" si="34"/>
-        <v>1637.2777538987559</v>
+        <v>993.04260436390462</v>
       </c>
       <c r="BL20" s="55">
         <f t="shared" si="34"/>
-        <v>1653.6505314377434</v>
+        <v>983.11217832026557</v>
       </c>
       <c r="BM20" s="55">
         <f t="shared" si="34"/>
-        <v>1670.1870367521208</v>
+        <v>973.28105653706291</v>
       </c>
       <c r="BN20" s="55">
         <f t="shared" si="34"/>
-        <v>1686.888907119642</v>
+        <v>963.54824597169227</v>
       </c>
       <c r="BO20" s="55">
         <f t="shared" si="34"/>
-        <v>1703.7577961908385</v>
+        <v>953.9127635119753</v>
       </c>
       <c r="BP20" s="55">
         <f t="shared" si="34"/>
-        <v>1720.7953741527469</v>
+        <v>944.37363587685559</v>
       </c>
       <c r="BQ20" s="55">
         <f t="shared" si="34"/>
-        <v>1738.0033278942744</v>
+        <v>934.92989951808704</v>
       </c>
       <c r="BR20" s="55">
         <f t="shared" si="34"/>
-        <v>1755.3833611732173</v>
+        <v>925.58060052290614</v>
       </c>
     </row>
     <row r="21" spans="2:70" x14ac:dyDescent="0.2">
@@ -8314,7 +8314,7 @@
         <v>824</v>
       </c>
       <c r="AO24" s="88">
-        <v>0.01</v>
+        <v>-0.01</v>
       </c>
       <c r="AP24" s="58"/>
       <c r="AQ24" s="58"/>
@@ -8647,7 +8647,7 @@
       </c>
       <c r="AO27" s="92">
         <f>NPV(AO25,AB20:BR20)</f>
-        <v>12008.558929838589</v>
+        <v>10684.690065769553</v>
       </c>
       <c r="AP27" s="54"/>
       <c r="AQ27" s="54"/>
@@ -8670,7 +8670,7 @@
       </c>
       <c r="AO29" s="93">
         <f>AO27+AO28</f>
-        <v>12385.137929838589</v>
+        <v>11061.269065769553</v>
       </c>
     </row>
     <row r="30" spans="2:70" x14ac:dyDescent="0.2">
@@ -8798,7 +8798,7 @@
       </c>
       <c r="AO30" s="95">
         <f>AO29/Main!C7</f>
-        <v>27.018189201218565</v>
+        <v>24.130168119043528</v>
       </c>
     </row>
     <row r="31" spans="2:70" x14ac:dyDescent="0.2">
@@ -8926,7 +8926,7 @@
       </c>
       <c r="AO31" s="97">
         <f>Main!C6</f>
-        <v>6.69</v>
+        <v>6.48</v>
       </c>
     </row>
     <row r="32" spans="2:70" x14ac:dyDescent="0.2">
@@ -9054,7 +9054,7 @@
       </c>
       <c r="AO32" s="99">
         <f>AO30/AO31-1</f>
-        <v>3.0385933036201145</v>
+        <v>2.7237913763956061</v>
       </c>
     </row>
     <row r="33" spans="2:41" x14ac:dyDescent="0.2">
@@ -9188,12 +9188,18 @@
       <c r="B37" s="68" t="s">
         <v>794</v>
       </c>
+      <c r="J37" s="32">
+        <v>172</v>
+      </c>
       <c r="K37" s="32">
         <v>176</v>
       </c>
       <c r="M37" s="32">
         <v>178</v>
       </c>
+      <c r="N37" s="32">
+        <v>179</v>
+      </c>
       <c r="O37" s="32">
         <v>180</v>
       </c>
@@ -9202,17 +9208,23 @@
       </c>
       <c r="R37" s="75"/>
       <c r="AB37" s="75"/>
-      <c r="AK37" s="121"/>
+      <c r="AK37" s="101"/>
     </row>
     <row r="38" spans="2:41" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B38" s="68" t="s">
         <v>795</v>
       </c>
+      <c r="J38" s="32">
+        <v>18</v>
+      </c>
       <c r="K38" s="32">
         <v>18</v>
       </c>
       <c r="M38" s="32">
         <v>17</v>
+      </c>
+      <c r="N38" s="32">
+        <v>18</v>
       </c>
       <c r="O38" s="32">
         <v>19</v>
@@ -9228,6 +9240,10 @@
       <c r="B39" s="67" t="s">
         <v>796</v>
       </c>
+      <c r="J39" s="32">
+        <f>J37+J38</f>
+        <v>190</v>
+      </c>
       <c r="K39" s="32">
         <f>K37+K38</f>
         <v>194</v>
@@ -9236,6 +9252,10 @@
         <f>M37+M38</f>
         <v>195</v>
       </c>
+      <c r="N39" s="32">
+        <f>N37+N38</f>
+        <v>197</v>
+      </c>
       <c r="O39" s="32">
         <f>O37+O38</f>
         <v>199</v>
@@ -9251,11 +9271,17 @@
       <c r="B40" s="68" t="s">
         <v>797</v>
       </c>
+      <c r="J40" s="32">
+        <v>122</v>
+      </c>
       <c r="K40" s="32">
         <v>134</v>
       </c>
       <c r="M40" s="32">
         <v>137</v>
+      </c>
+      <c r="N40" s="32">
+        <v>144</v>
       </c>
       <c r="O40" s="32">
         <v>144</v>
@@ -9270,10 +9296,16 @@
       <c r="B41" s="68" t="s">
         <v>798</v>
       </c>
+      <c r="J41" s="32">
+        <v>116</v>
+      </c>
       <c r="K41" s="32">
         <v>111</v>
       </c>
       <c r="M41" s="32">
+        <v>95</v>
+      </c>
+      <c r="N41" s="32">
         <v>95</v>
       </c>
       <c r="O41" s="32">
@@ -9289,6 +9321,10 @@
       <c r="B42" s="67" t="s">
         <v>799</v>
       </c>
+      <c r="J42" s="32">
+        <f>J40+J41</f>
+        <v>238</v>
+      </c>
       <c r="K42" s="32">
         <f>K40+K41</f>
         <v>245</v>
@@ -9297,6 +9333,10 @@
         <f>M40+M41</f>
         <v>232</v>
       </c>
+      <c r="N42" s="32">
+        <f>N40+N41</f>
+        <v>239</v>
+      </c>
       <c r="O42" s="32">
         <f>O40+O41</f>
         <v>223</v>
@@ -9312,6 +9352,9 @@
       <c r="B43" s="51" t="s">
         <v>802</v>
       </c>
+      <c r="J43" s="1">
+        <v>294</v>
+      </c>
       <c r="K43" s="32">
         <f>K37+K40</f>
         <v>310</v>
@@ -9320,6 +9363,9 @@
         <f>M37+M40</f>
         <v>315</v>
       </c>
+      <c r="N43" s="1">
+        <v>323</v>
+      </c>
       <c r="O43" s="32">
         <f>O37+O40</f>
         <v>324</v>
@@ -9333,6 +9379,9 @@
       <c r="B44" s="51" t="s">
         <v>801</v>
       </c>
+      <c r="J44" s="1">
+        <v>134</v>
+      </c>
       <c r="K44" s="1">
         <f>K38+K41</f>
         <v>129</v>
@@ -9341,6 +9390,9 @@
         <f>M38+M41</f>
         <v>112</v>
       </c>
+      <c r="N44" s="1">
+        <v>113</v>
+      </c>
       <c r="O44" s="1">
         <f>O38+O41</f>
         <v>98</v>
@@ -9354,6 +9406,10 @@
       <c r="B45" s="2" t="s">
         <v>800</v>
       </c>
+      <c r="J45" s="58">
+        <f>J43+J44</f>
+        <v>428</v>
+      </c>
       <c r="K45" s="58">
         <f>K43+K44</f>
         <v>439</v>
@@ -9362,6 +9418,10 @@
         <f>M43+M44</f>
         <v>427</v>
       </c>
+      <c r="N45" s="58">
+        <f>N43+N44</f>
+        <v>436</v>
+      </c>
       <c r="O45" s="58">
         <f>O43+O44</f>
         <v>422</v>
@@ -9385,6 +9445,10 @@
     <row r="47" spans="2:41" x14ac:dyDescent="0.2">
       <c r="B47" s="1" t="s">
         <v>814</v>
+      </c>
+      <c r="J47" s="53">
+        <f>J6/J45</f>
+        <v>3.2027757009345796</v>
       </c>
       <c r="K47" s="53">
         <f>K6/K45</f>
@@ -9395,7 +9459,10 @@
         <f>M6/M45</f>
         <v>3.1108594847775177</v>
       </c>
-      <c r="N47" s="53"/>
+      <c r="N47" s="53">
+        <f>N6/N45</f>
+        <v>3.4731513761467894</v>
+      </c>
       <c r="O47" s="53">
         <f>O6/O45</f>
         <v>3.5264336492891002</v>
@@ -9427,8 +9494,14 @@
       <c r="B50" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="J50" s="21">
+        <v>865.60900000000004</v>
+      </c>
       <c r="K50" s="21">
         <v>1517.3610000000001</v>
+      </c>
+      <c r="N50" s="21">
+        <v>1253.7059999999999</v>
       </c>
       <c r="O50" s="21">
         <v>1669.453</v>
@@ -9471,8 +9544,14 @@
       <c r="B51" s="1" t="s">
         <v>89</v>
       </c>
+      <c r="J51" s="22">
+        <v>806.91600000000005</v>
+      </c>
       <c r="K51" s="22">
         <v>527.34</v>
+      </c>
+      <c r="N51" s="22">
+        <v>735.779</v>
       </c>
       <c r="O51" s="22">
         <v>569.01400000000001</v>
@@ -9495,8 +9574,14 @@
       <c r="B52" s="2" t="s">
         <v>90</v>
       </c>
+      <c r="J52" s="21">
+        <v>1056.845</v>
+      </c>
       <c r="K52" s="21">
         <v>895.97400000000005</v>
+      </c>
+      <c r="N52" s="21">
+        <v>837.74</v>
       </c>
       <c r="O52" s="21">
         <v>811.41</v>
@@ -9539,8 +9624,14 @@
       <c r="B53" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="J53" s="22">
+        <v>243.971</v>
+      </c>
       <c r="K53" s="22">
         <v>282.3</v>
+      </c>
+      <c r="N53" s="22">
+        <v>300.71899999999999</v>
       </c>
       <c r="O53" s="22">
         <v>286.42200000000003</v>
@@ -9572,8 +9663,8 @@
         <v>0</v>
       </c>
       <c r="J54" s="22">
-        <f t="shared" si="77"/>
-        <v>0</v>
+        <f>SUM(J50:J53)</f>
+        <v>2973.3409999999999</v>
       </c>
       <c r="K54" s="22">
         <f t="shared" si="77"/>
@@ -9589,7 +9680,7 @@
       </c>
       <c r="N54" s="22">
         <f t="shared" si="77"/>
-        <v>0</v>
+        <v>3127.944</v>
       </c>
       <c r="O54" s="22">
         <f>SUM(O50:O53)</f>
@@ -9616,8 +9707,14 @@
       <c r="B55" s="1" t="s">
         <v>93</v>
       </c>
+      <c r="J55" s="22">
+        <v>680.87099999999998</v>
+      </c>
       <c r="K55" s="22">
         <v>658.678</v>
+      </c>
+      <c r="N55" s="22">
+        <v>601.70000000000005</v>
       </c>
       <c r="O55" s="22">
         <v>607.226</v>
@@ -9640,8 +9737,14 @@
       <c r="B56" s="1" t="s">
         <v>94</v>
       </c>
+      <c r="J56" s="22">
+        <v>560.14599999999996</v>
+      </c>
       <c r="K56" s="22">
         <v>536.66</v>
+      </c>
+      <c r="N56" s="22">
+        <v>469.63799999999998</v>
       </c>
       <c r="O56" s="22">
         <v>448.36399999999998</v>
@@ -9664,10 +9767,18 @@
       <c r="B57" s="1" t="s">
         <v>95</v>
       </c>
+      <c r="J57" s="22">
+        <f>493.631+37.274</f>
+        <v>530.90499999999997</v>
+      </c>
       <c r="K57" s="22">
         <f>502.214+13.295</f>
         <v>515.50900000000001</v>
       </c>
+      <c r="N57" s="22">
+        <f>498.166+11.474</f>
+        <v>509.64</v>
+      </c>
       <c r="O57" s="22">
         <f>495.215+11.01</f>
         <v>506.22499999999997</v>
@@ -9693,8 +9804,14 @@
       <c r="B58" s="1" t="s">
         <v>96</v>
       </c>
+      <c r="J58" s="22">
+        <v>45.994999999999997</v>
+      </c>
       <c r="K58" s="22">
         <v>23.93</v>
+      </c>
+      <c r="N58" s="22">
+        <v>34.542999999999999</v>
       </c>
       <c r="O58" s="22">
         <v>17.812000000000001</v>
@@ -9717,8 +9834,14 @@
       <c r="B59" s="1" t="s">
         <v>97</v>
       </c>
+      <c r="J59" s="22">
+        <v>72.293000000000006</v>
+      </c>
       <c r="K59" s="22">
         <v>72.876000000000005</v>
+      </c>
+      <c r="N59" s="22">
+        <v>78.835999999999999</v>
       </c>
       <c r="O59" s="22">
         <v>75.47</v>
@@ -9751,7 +9874,7 @@
       </c>
       <c r="J60" s="22">
         <f t="shared" si="79"/>
-        <v>0</v>
+        <v>4863.5509999999995</v>
       </c>
       <c r="K60" s="22">
         <f t="shared" si="79"/>
@@ -9767,7 +9890,7 @@
       </c>
       <c r="N60" s="22">
         <f t="shared" si="79"/>
-        <v>0</v>
+        <v>4822.3010000000004</v>
       </c>
       <c r="O60" s="22">
         <f>O54+O55+O56+O57+O58+O59</f>
@@ -9800,8 +9923,14 @@
       <c r="B62" s="1" t="s">
         <v>99</v>
       </c>
+      <c r="J62" s="22">
+        <v>643.31500000000005</v>
+      </c>
       <c r="K62" s="22">
         <v>575.95399999999995</v>
+      </c>
+      <c r="N62" s="22">
+        <v>532.91899999999998</v>
       </c>
       <c r="O62" s="22">
         <v>613.30700000000002</v>
@@ -9824,8 +9953,14 @@
       <c r="B63" s="1" t="s">
         <v>100</v>
       </c>
+      <c r="J63" s="22">
+        <v>309.096</v>
+      </c>
       <c r="K63" s="22">
         <v>378.85899999999998</v>
+      </c>
+      <c r="N63" s="22">
+        <v>388.27499999999998</v>
       </c>
       <c r="O63" s="22">
         <v>460.16500000000002</v>
@@ -9848,8 +9983,14 @@
       <c r="B64" s="1" t="s">
         <v>101</v>
       </c>
+      <c r="J64" s="22">
+        <v>197.49600000000001</v>
+      </c>
       <c r="K64" s="22">
         <v>203.399</v>
+      </c>
+      <c r="N64" s="22">
+        <v>174.274</v>
       </c>
       <c r="O64" s="22">
         <v>164.29400000000001</v>
@@ -9872,8 +10013,14 @@
       <c r="B65" s="1" t="s">
         <v>102</v>
       </c>
+      <c r="J65" s="22">
+        <v>156.88499999999999</v>
+      </c>
       <c r="K65" s="22">
         <v>162.56100000000001</v>
+      </c>
+      <c r="N65" s="22">
+        <v>142.566</v>
       </c>
       <c r="O65" s="22">
         <v>138.684</v>
@@ -9896,8 +10043,14 @@
       <c r="B66" s="1" t="s">
         <v>103</v>
       </c>
+      <c r="J66" s="22">
+        <v>141.607</v>
+      </c>
       <c r="K66" s="22">
         <v>92.503</v>
+      </c>
+      <c r="N66" s="22">
+        <v>116.504</v>
       </c>
       <c r="O66" s="22">
         <v>73.745999999999995</v>
@@ -9930,7 +10083,7 @@
       </c>
       <c r="J67" s="22">
         <f t="shared" si="81"/>
-        <v>0</v>
+        <v>1448.3990000000001</v>
       </c>
       <c r="K67" s="22">
         <f t="shared" si="81"/>
@@ -9946,7 +10099,7 @@
       </c>
       <c r="N67" s="22">
         <f t="shared" si="81"/>
-        <v>0</v>
+        <v>1354.5379999999998</v>
       </c>
       <c r="O67" s="22">
         <f>SUM(O62:O66)</f>
@@ -9973,8 +10126,14 @@
       <c r="B68" s="2" t="s">
         <v>105</v>
       </c>
+      <c r="J68" s="21">
+        <v>997.34699999999998</v>
+      </c>
       <c r="K68" s="21">
         <v>1003.556</v>
+      </c>
+      <c r="N68" s="21">
+        <v>662.90300000000002</v>
       </c>
       <c r="O68" s="21">
         <v>662.53099999999995</v>
@@ -10017,8 +10176,14 @@
       <c r="B69" s="1" t="s">
         <v>102</v>
       </c>
+      <c r="J69" s="22">
+        <v>872.79100000000005</v>
+      </c>
       <c r="K69" s="22">
         <v>839.41399999999999</v>
+      </c>
+      <c r="N69" s="22">
+        <v>728.077</v>
       </c>
       <c r="O69" s="22">
         <v>703.11099999999999</v>
@@ -10041,8 +10206,14 @@
       <c r="B70" s="1" t="s">
         <v>106</v>
       </c>
+      <c r="J70" s="22">
+        <v>74.668000000000006</v>
+      </c>
       <c r="K70" s="22">
         <v>98.388999999999996</v>
+      </c>
+      <c r="N70" s="22">
+        <v>99.034000000000006</v>
       </c>
       <c r="O70" s="22">
         <v>86.584000000000003</v>
@@ -10075,7 +10246,7 @@
       </c>
       <c r="J71" s="22">
         <f t="shared" si="82"/>
-        <v>0</v>
+        <v>3393.2050000000004</v>
       </c>
       <c r="K71" s="22">
         <f t="shared" si="82"/>
@@ -10091,7 +10262,7 @@
       </c>
       <c r="N71" s="22">
         <f t="shared" si="82"/>
-        <v>0</v>
+        <v>2844.5520000000001</v>
       </c>
       <c r="O71" s="22">
         <f>O67+O68+O69+O70</f>
@@ -10123,8 +10294,14 @@
       <c r="B73" s="1" t="s">
         <v>108</v>
       </c>
+      <c r="J73" s="22">
+        <v>1470.346</v>
+      </c>
       <c r="K73" s="22">
         <v>1675.9929999999999</v>
+      </c>
+      <c r="N73" s="22">
+        <v>1977.749</v>
       </c>
       <c r="O73" s="22">
         <v>2088.9940000000001</v>
@@ -10147,10 +10324,18 @@
       <c r="B74" s="1" t="s">
         <v>109</v>
       </c>
+      <c r="J74" s="22">
+        <f>J71+J73</f>
+        <v>4863.5510000000004</v>
+      </c>
       <c r="K74" s="22">
         <f>K71+K73</f>
         <v>5030.6280000000006</v>
       </c>
+      <c r="N74" s="22">
+        <f>N71+N73</f>
+        <v>4822.3010000000004</v>
+      </c>
       <c r="O74" s="22">
         <f>O71+O73</f>
         <v>4991.4159999999993</v>
@@ -10176,12 +10361,20 @@
       <c r="B76" s="1" t="s">
         <v>777</v>
       </c>
+      <c r="J76" s="22">
+        <f t="shared" ref="J76:K76" si="84">J60-J71</f>
+        <v>1470.3459999999991</v>
+      </c>
       <c r="K76" s="22">
-        <f t="shared" ref="K76" si="84">K60-K71</f>
+        <f t="shared" si="84"/>
         <v>1675.9930000000004</v>
       </c>
+      <c r="N76" s="22">
+        <f t="shared" ref="N76:O76" si="85">N60-N71</f>
+        <v>1977.7490000000003</v>
+      </c>
       <c r="O76" s="22">
-        <f t="shared" ref="O76" si="85">O60-O71</f>
+        <f t="shared" si="85"/>
         <v>2088.9740000000011</v>
       </c>
       <c r="P76" s="22">
@@ -10205,12 +10398,20 @@
       <c r="B77" s="1" t="s">
         <v>776</v>
       </c>
+      <c r="J77" s="53">
+        <f t="shared" ref="J77:K77" si="87">J76/J22</f>
+        <v>3.2196840634675921</v>
+      </c>
       <c r="K77" s="53">
-        <f t="shared" ref="K77" si="87">K76/K22</f>
+        <f t="shared" si="87"/>
         <v>3.6850318044198591</v>
       </c>
+      <c r="N77" s="53">
+        <f t="shared" ref="N77:O77" si="88">N76/N22</f>
+        <v>4.2079586895374916</v>
+      </c>
       <c r="O77" s="53">
-        <f t="shared" ref="O77" si="88">O76/O22</f>
+        <f t="shared" si="88"/>
         <v>4.3869603383608675</v>
       </c>
       <c r="P77" s="53">
@@ -10233,6 +10434,10 @@
     <row r="79" spans="2:46" s="58" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B79" s="58" t="s">
         <v>790</v>
+      </c>
+      <c r="N79" s="70">
+        <f>N52/J52-1</f>
+        <v>-0.20731990026919744</v>
       </c>
       <c r="O79" s="70">
         <f>O52/K52-1</f>
@@ -10249,8 +10454,16 @@
       <c r="B80" s="32" t="s">
         <v>791</v>
       </c>
+      <c r="K80" s="65">
+        <f t="shared" ref="K80" si="89">K52/J52-1</f>
+        <v>-0.15221815876500333</v>
+      </c>
+      <c r="O80" s="65">
+        <f t="shared" ref="O80" si="90">O52/N52-1</f>
+        <v>-3.1429799221715626E-2</v>
+      </c>
       <c r="P80" s="65">
-        <f t="shared" ref="P80" si="89">P52/O52-1</f>
+        <f t="shared" ref="P80" si="91">P52/O52-1</f>
         <v>1.6076952465461369E-2</v>
       </c>
       <c r="Q80" s="65">
@@ -10265,39 +10478,39 @@
         <v>6</v>
       </c>
       <c r="H82" s="56">
-        <f t="shared" ref="H82:N82" si="90">H50</f>
+        <f t="shared" ref="H82:N82" si="92">H50</f>
         <v>0</v>
       </c>
       <c r="I82" s="56">
-        <f t="shared" si="90"/>
+        <f t="shared" si="92"/>
         <v>0</v>
       </c>
       <c r="J82" s="56">
-        <f t="shared" si="90"/>
+        <f t="shared" ref="J82:K82" si="93">J50</f>
+        <v>865.60900000000004</v>
+      </c>
+      <c r="K82" s="56">
+        <f t="shared" si="92"/>
+        <v>1517.3610000000001</v>
+      </c>
+      <c r="L82" s="56">
+        <f t="shared" si="92"/>
         <v>0</v>
       </c>
-      <c r="K82" s="56">
-        <f t="shared" si="90"/>
-        <v>1517.3610000000001</v>
-      </c>
-      <c r="L82" s="56">
-        <f t="shared" si="90"/>
+      <c r="M82" s="56">
+        <f t="shared" si="92"/>
         <v>0</v>
       </c>
-      <c r="M82" s="56">
-        <f t="shared" si="90"/>
-        <v>0</v>
-      </c>
       <c r="N82" s="56">
-        <f t="shared" si="90"/>
-        <v>0</v>
+        <f t="shared" si="92"/>
+        <v>1253.7059999999999</v>
       </c>
       <c r="O82" s="56">
-        <f t="shared" ref="O82:P82" si="91">O50</f>
+        <f t="shared" ref="O82:P82" si="94">O50</f>
         <v>1669.453</v>
       </c>
       <c r="P82" s="56">
-        <f t="shared" si="91"/>
+        <f t="shared" si="94"/>
         <v>1009.139</v>
       </c>
       <c r="Q82" s="56">
@@ -10306,11 +10519,11 @@
       </c>
       <c r="R82" s="74"/>
       <c r="Z82" s="56">
-        <f t="shared" ref="Z82:AA82" si="92">Z50</f>
+        <f t="shared" ref="Z82:AA82" si="95">Z50</f>
         <v>1517.3610000000001</v>
       </c>
       <c r="AA82" s="56">
-        <f t="shared" si="92"/>
+        <f t="shared" si="95"/>
         <v>1669.453</v>
       </c>
       <c r="AB82" s="75"/>
@@ -10320,39 +10533,39 @@
         <v>7</v>
       </c>
       <c r="H83" s="56">
-        <f t="shared" ref="H83:N83" si="93">H68</f>
+        <f t="shared" ref="H83:N83" si="96">H68</f>
         <v>0</v>
       </c>
       <c r="I83" s="56">
-        <f t="shared" si="93"/>
+        <f t="shared" si="96"/>
         <v>0</v>
       </c>
       <c r="J83" s="56">
-        <f t="shared" si="93"/>
+        <f t="shared" ref="J83:K83" si="97">J68</f>
+        <v>997.34699999999998</v>
+      </c>
+      <c r="K83" s="56">
+        <f t="shared" si="96"/>
+        <v>1003.556</v>
+      </c>
+      <c r="L83" s="56">
+        <f t="shared" si="96"/>
         <v>0</v>
       </c>
-      <c r="K83" s="56">
-        <f t="shared" si="93"/>
-        <v>1003.556</v>
-      </c>
-      <c r="L83" s="56">
-        <f t="shared" si="93"/>
+      <c r="M83" s="56">
+        <f t="shared" si="96"/>
         <v>0</v>
       </c>
-      <c r="M83" s="56">
-        <f t="shared" si="93"/>
-        <v>0</v>
-      </c>
       <c r="N83" s="56">
-        <f t="shared" si="93"/>
-        <v>0</v>
+        <f t="shared" si="96"/>
+        <v>662.90300000000002</v>
       </c>
       <c r="O83" s="56">
-        <f t="shared" ref="O83:P83" si="94">O68</f>
+        <f t="shared" ref="O83:P83" si="98">O68</f>
         <v>662.53099999999995</v>
       </c>
       <c r="P83" s="56">
-        <f t="shared" si="94"/>
+        <f t="shared" si="98"/>
         <v>672.28599999999994</v>
       </c>
       <c r="Q83" s="56">
@@ -10361,11 +10574,11 @@
       </c>
       <c r="R83" s="74"/>
       <c r="Z83" s="56">
-        <f t="shared" ref="Z83:AA83" si="95">Z68</f>
+        <f t="shared" ref="Z83:AA83" si="99">Z68</f>
         <v>1003.556</v>
       </c>
       <c r="AA83" s="56">
-        <f t="shared" si="95"/>
+        <f t="shared" si="99"/>
         <v>662.53099999999995</v>
       </c>
       <c r="AB83" s="75"/>
@@ -10375,39 +10588,39 @@
         <v>8</v>
       </c>
       <c r="H84" s="22">
-        <f t="shared" ref="H84:N84" si="96">H82-H83</f>
+        <f t="shared" ref="H84:N84" si="100">H82-H83</f>
         <v>0</v>
       </c>
       <c r="I84" s="22">
-        <f t="shared" si="96"/>
+        <f t="shared" si="100"/>
         <v>0</v>
       </c>
       <c r="J84" s="22">
-        <f t="shared" si="96"/>
+        <f t="shared" ref="J84:K84" si="101">J82-J83</f>
+        <v>-131.73799999999994</v>
+      </c>
+      <c r="K84" s="22">
+        <f t="shared" si="100"/>
+        <v>513.80500000000006</v>
+      </c>
+      <c r="L84" s="22">
+        <f t="shared" si="100"/>
         <v>0</v>
       </c>
-      <c r="K84" s="22">
-        <f t="shared" si="96"/>
-        <v>513.80500000000006</v>
-      </c>
-      <c r="L84" s="22">
-        <f t="shared" si="96"/>
+      <c r="M84" s="22">
+        <f t="shared" si="100"/>
         <v>0</v>
       </c>
-      <c r="M84" s="22">
-        <f t="shared" si="96"/>
-        <v>0</v>
-      </c>
       <c r="N84" s="22">
-        <f t="shared" si="96"/>
-        <v>0</v>
+        <f t="shared" si="100"/>
+        <v>590.80299999999988</v>
       </c>
       <c r="O84" s="22">
-        <f t="shared" ref="O84:P84" si="97">O82-O83</f>
+        <f t="shared" ref="O84:P84" si="102">O82-O83</f>
         <v>1006.922</v>
       </c>
       <c r="P84" s="22">
-        <f t="shared" si="97"/>
+        <f t="shared" si="102"/>
         <v>336.85300000000007</v>
       </c>
       <c r="Q84" s="22">
@@ -10416,11 +10629,11 @@
       </c>
       <c r="R84" s="74"/>
       <c r="Z84" s="22">
-        <f t="shared" ref="Z84:AA84" si="98">Z82-Z83</f>
+        <f t="shared" ref="Z84:AA84" si="103">Z82-Z83</f>
         <v>513.80500000000006</v>
       </c>
       <c r="AA84" s="22">
-        <f t="shared" si="98"/>
+        <f t="shared" si="103"/>
         <v>1006.922</v>
       </c>
     </row>
@@ -10491,64 +10704,64 @@
         <v>3808.6451099999999</v>
       </c>
       <c r="I87" s="56">
-        <f t="shared" ref="I87:Q87" si="99">I86*I22</f>
+        <f t="shared" ref="I87:Q87" si="104">I86*I22</f>
         <v>4014.4296399999998</v>
       </c>
       <c r="J87" s="56">
-        <f t="shared" si="99"/>
+        <f t="shared" si="104"/>
         <v>4493.6721600000001</v>
       </c>
       <c r="K87" s="56">
-        <f t="shared" si="99"/>
+        <f t="shared" si="104"/>
         <v>6767.5876799999996</v>
       </c>
       <c r="L87" s="56">
-        <f t="shared" si="99"/>
+        <f t="shared" si="104"/>
         <v>8418.0184399999998</v>
       </c>
       <c r="M87" s="56">
-        <f t="shared" si="99"/>
+        <f t="shared" si="104"/>
         <v>8534.8462799999998</v>
       </c>
       <c r="N87" s="56">
-        <f t="shared" si="99"/>
+        <f t="shared" si="104"/>
         <v>8234.4350400000003</v>
       </c>
       <c r="O87" s="56">
-        <f t="shared" si="99"/>
+        <f t="shared" si="104"/>
         <v>8590.251119999999</v>
       </c>
       <c r="P87" s="56">
-        <f t="shared" si="99"/>
+        <f t="shared" si="104"/>
         <v>7580.5139999999992</v>
       </c>
       <c r="Q87" s="56">
-        <f t="shared" si="99"/>
+        <f t="shared" si="104"/>
         <v>3474.7857000000004</v>
       </c>
       <c r="R87" s="75"/>
       <c r="V87" s="56">
-        <f t="shared" ref="V87:Y87" si="100">V86*V22</f>
+        <f t="shared" ref="V87:Y87" si="105">V86*V22</f>
         <v>10982.426100000001</v>
       </c>
       <c r="W87" s="56">
-        <f t="shared" si="100"/>
+        <f t="shared" si="105"/>
         <v>5870.5102799999995</v>
       </c>
       <c r="X87" s="56">
-        <f t="shared" si="100"/>
+        <f t="shared" si="105"/>
         <v>7208.8285500000011</v>
       </c>
       <c r="Y87" s="56">
-        <f t="shared" si="100"/>
+        <f t="shared" si="105"/>
         <v>8649.4895199999992</v>
       </c>
       <c r="Z87" s="56">
-        <f t="shared" ref="Z87:AA87" si="101">Z86*Z22</f>
+        <f t="shared" ref="Z87:AA87" si="106">Z86*Z22</f>
         <v>6756.8443200000002</v>
       </c>
       <c r="AA87" s="56">
-        <f t="shared" si="101"/>
+        <f t="shared" si="106"/>
         <v>8397.6921600000005</v>
       </c>
       <c r="AB87" s="75"/>
@@ -10557,16 +10770,24 @@
       <c r="B88" s="56" t="s">
         <v>9</v>
       </c>
+      <c r="J88" s="56">
+        <f t="shared" ref="J88:N88" si="107">J87-J84</f>
+        <v>4625.4101600000004</v>
+      </c>
       <c r="K88" s="56">
-        <f t="shared" ref="K88" si="102">K87-K84</f>
+        <f t="shared" si="107"/>
         <v>6253.7826799999993</v>
       </c>
+      <c r="N88" s="56">
+        <f t="shared" si="107"/>
+        <v>7643.6320400000004</v>
+      </c>
       <c r="O88" s="56">
-        <f t="shared" ref="O88:P88" si="103">O87-O84</f>
+        <f t="shared" ref="O88:P88" si="108">O87-O84</f>
         <v>7583.3291199999985</v>
       </c>
       <c r="P88" s="56">
-        <f t="shared" si="103"/>
+        <f t="shared" si="108"/>
         <v>7243.6609999999991</v>
       </c>
       <c r="Q88" s="56">
@@ -10575,11 +10796,11 @@
       </c>
       <c r="R88" s="74"/>
       <c r="Z88" s="56">
-        <f t="shared" ref="Z88:AA88" si="104">Z87-Z84</f>
+        <f t="shared" ref="Z88:AA88" si="109">Z87-Z84</f>
         <v>6243.0393199999999</v>
       </c>
       <c r="AA88" s="56">
-        <f t="shared" si="104"/>
+        <f t="shared" si="109"/>
         <v>7390.77016</v>
       </c>
       <c r="AB88" s="74"/>
@@ -10588,16 +10809,24 @@
       <c r="B90" s="1" t="s">
         <v>778</v>
       </c>
+      <c r="J90" s="69">
+        <f t="shared" ref="J90:K90" si="110">J86/J77</f>
+        <v>3.0562004861440792</v>
+      </c>
       <c r="K90" s="69">
-        <f t="shared" ref="K90" si="105">K86/K77</f>
+        <f t="shared" si="110"/>
         <v>4.0379570081736604</v>
       </c>
+      <c r="N90" s="69">
+        <f t="shared" ref="N90:P90" si="111">N86/N77</f>
+        <v>4.1635389728423569</v>
+      </c>
       <c r="O90" s="69">
-        <f t="shared" ref="O90:P90" si="106">O86/O77</f>
+        <f t="shared" si="111"/>
         <v>4.1121867098393734</v>
       </c>
       <c r="P90" s="69">
-        <f t="shared" si="106"/>
+        <f t="shared" si="111"/>
         <v>4.3844509454849581</v>
       </c>
       <c r="Q90" s="69">
@@ -10605,7 +10834,7 @@
         <v>2.0095979110459519</v>
       </c>
       <c r="Z90" s="69">
-        <f t="shared" ref="Z90" si="107">Z86/Z77</f>
+        <f t="shared" ref="Z90" si="112">Z86/Z77</f>
         <v>4.0379570081736604</v>
       </c>
       <c r="AA90" s="69">
@@ -10617,28 +10846,32 @@
       <c r="B91" s="1" t="s">
         <v>809</v>
       </c>
+      <c r="J91" s="69">
+        <f t="shared" ref="J91" si="113">J87/SUM(G6:J6)</f>
+        <v>1.5423293411981622</v>
+      </c>
       <c r="K91" s="69">
-        <f t="shared" ref="K91:P91" si="108">K87/SUM(H6:K6)</f>
+        <f t="shared" ref="K91:P91" si="114">K87/SUM(H6:K6)</f>
         <v>1.5995330818390172</v>
       </c>
       <c r="L91" s="69">
-        <f t="shared" si="108"/>
+        <f t="shared" si="114"/>
         <v>1.8332967691100841</v>
       </c>
       <c r="M91" s="69">
-        <f t="shared" si="108"/>
+        <f t="shared" si="114"/>
         <v>1.6247491502037685</v>
       </c>
       <c r="N91" s="69">
-        <f t="shared" si="108"/>
+        <f t="shared" si="114"/>
         <v>1.5258758943246864</v>
       </c>
       <c r="O91" s="69">
-        <f t="shared" si="108"/>
+        <f t="shared" si="114"/>
         <v>1.5429916494080578</v>
       </c>
       <c r="P91" s="69">
-        <f t="shared" si="108"/>
+        <f t="shared" si="114"/>
         <v>1.3534483543594595</v>
       </c>
       <c r="Q91" s="69">
@@ -10646,23 +10879,23 @@
         <v>0.6221570503604078</v>
       </c>
       <c r="V91" s="69">
-        <f t="shared" ref="V91:Y91" si="109">V87/V6</f>
+        <f t="shared" ref="V91:Y91" si="115">V87/V6</f>
         <v>2.3621676596476893</v>
       </c>
       <c r="W91" s="69">
-        <f t="shared" si="109"/>
+        <f t="shared" si="115"/>
         <v>1.2305088267185433</v>
       </c>
       <c r="X91" s="69">
-        <f t="shared" si="109"/>
+        <f t="shared" si="115"/>
         <v>1.456904992539475</v>
       </c>
       <c r="Y91" s="69">
-        <f t="shared" si="109"/>
+        <f t="shared" si="115"/>
         <v>1.7392236210561027</v>
       </c>
       <c r="Z91" s="69">
-        <f t="shared" ref="Z91" si="110">Z87/Z6</f>
+        <f t="shared" ref="Z91" si="116">Z87/Z6</f>
         <v>1.5969938669011909</v>
       </c>
       <c r="AA91" s="69">
@@ -10674,28 +10907,32 @@
       <c r="B92" s="1" t="s">
         <v>58</v>
       </c>
+      <c r="J92" s="69">
+        <f t="shared" ref="J92" si="117">J86/SUM(G21:J21)</f>
+        <v>-6.0757314053217959</v>
+      </c>
       <c r="K92" s="69">
-        <f t="shared" ref="K92" si="111">K86/SUM(H21:K21)</f>
+        <f t="shared" ref="K92" si="118">K86/SUM(H21:K21)</f>
         <v>-12.257039736665067</v>
       </c>
       <c r="L92" s="69">
-        <f t="shared" ref="L92" si="112">L86/SUM(I21:L21)</f>
+        <f t="shared" ref="L92" si="119">L86/SUM(I21:L21)</f>
         <v>71.383779306426774</v>
       </c>
       <c r="M92" s="69">
-        <f t="shared" ref="M92" si="113">M86/SUM(J21:M21)</f>
+        <f t="shared" ref="M92" si="120">M86/SUM(J21:M21)</f>
         <v>18.285031241280244</v>
       </c>
       <c r="N92" s="69">
-        <f t="shared" ref="N92" si="114">N86/SUM(K21:N21)</f>
+        <f t="shared" ref="N92" si="121">N86/SUM(K21:N21)</f>
         <v>14.952988283370482</v>
       </c>
       <c r="O92" s="69">
-        <f t="shared" ref="O92:P92" si="115">O86/SUM(L21:O21)</f>
+        <f t="shared" ref="O92:P92" si="122">O86/SUM(L21:O21)</f>
         <v>18.105251010476522</v>
       </c>
       <c r="P92" s="69">
-        <f t="shared" si="115"/>
+        <f t="shared" si="122"/>
         <v>22.989620990664498</v>
       </c>
       <c r="Q92" s="69">
@@ -10703,23 +10940,23 @@
         <v>20.941179022554319</v>
       </c>
       <c r="V92" s="69">
-        <f t="shared" ref="V92:X92" si="116">V86/V21</f>
+        <f t="shared" ref="V92:X92" si="123">V86/V21</f>
         <v>42.458927163071316</v>
       </c>
       <c r="W92" s="69">
-        <f t="shared" si="116"/>
+        <f t="shared" si="123"/>
         <v>-121.64339577289637</v>
       </c>
       <c r="X92" s="69">
-        <f t="shared" si="116"/>
+        <f t="shared" si="123"/>
         <v>-155.69151548529089</v>
       </c>
       <c r="Y92" s="69">
-        <f t="shared" ref="Y92:Z92" si="117">Y86/Y21</f>
+        <f t="shared" ref="Y92:Z92" si="124">Y86/Y21</f>
         <v>93.871302120640664</v>
       </c>
       <c r="Z92" s="69">
-        <f t="shared" si="117"/>
+        <f t="shared" si="124"/>
         <v>-12.303582123796154</v>
       </c>
       <c r="AA92" s="69">
@@ -10732,7 +10969,7 @@
         <v>810</v>
       </c>
       <c r="Z93" s="69">
-        <f t="shared" ref="Z93" si="118">Z88/Z6</f>
+        <f t="shared" ref="Z93" si="125">Z88/Z6</f>
         <v>1.4755550124711148</v>
       </c>
       <c r="AA93" s="69">
@@ -10748,16 +10985,24 @@
       <c r="B95" s="1" t="s">
         <v>806</v>
       </c>
+      <c r="J95" s="25">
+        <f t="shared" ref="J95:K95" si="126">J52/J9</f>
+        <v>0.73749442611099214</v>
+      </c>
       <c r="K95" s="25">
-        <f t="shared" ref="K95" si="119">K52/K9</f>
+        <f t="shared" si="126"/>
         <v>0.63826449707429866</v>
       </c>
+      <c r="N95" s="25">
+        <f t="shared" ref="N95:P95" si="127">N52/N9</f>
+        <v>0.54203989305947731</v>
+      </c>
       <c r="O95" s="25">
-        <f t="shared" ref="O95:P95" si="120">O52/O9</f>
+        <f t="shared" si="127"/>
         <v>0.53060904195317171</v>
       </c>
       <c r="P95" s="25">
-        <f t="shared" si="120"/>
+        <f t="shared" si="127"/>
         <v>0.63373547690332799</v>
       </c>
       <c r="Q95" s="25">
@@ -10765,7 +11010,7 @@
         <v>0.70745268732158828</v>
       </c>
       <c r="Z95" s="25">
-        <f t="shared" ref="Z95" si="121">Z52/Z9</f>
+        <f t="shared" ref="Z95" si="128">Z52/Z9</f>
         <v>0.20023255361795636</v>
       </c>
       <c r="AA95" s="25">
@@ -10799,35 +11044,35 @@
         <v>815</v>
       </c>
       <c r="I100" s="65">
-        <f t="shared" ref="I100:P100" si="122">I3/H3-1</f>
+        <f t="shared" ref="I100:P100" si="129">I3/H3-1</f>
         <v>-0.28820449048700714</v>
       </c>
       <c r="J100" s="65">
-        <f t="shared" si="122"/>
+        <f t="shared" si="129"/>
         <v>1.1768782082290343</v>
       </c>
       <c r="K100" s="65">
-        <f t="shared" si="122"/>
+        <f t="shared" si="129"/>
         <v>4.6761685836980149E-3</v>
       </c>
       <c r="L100" s="65">
-        <f t="shared" si="122"/>
+        <f t="shared" si="129"/>
         <v>-0.13027499098108597</v>
       </c>
       <c r="M100" s="65">
-        <f t="shared" si="122"/>
+        <f t="shared" si="129"/>
         <v>7.9195991314019887E-2</v>
       </c>
       <c r="N100" s="65">
-        <f t="shared" si="122"/>
+        <f t="shared" si="129"/>
         <v>0.21052330549432452</v>
       </c>
       <c r="O100" s="65">
-        <f t="shared" si="122"/>
+        <f t="shared" si="129"/>
         <v>3.8321500693137889E-2</v>
       </c>
       <c r="P100" s="65">
-        <f t="shared" si="122"/>
+        <f t="shared" si="129"/>
         <v>-0.2022053470017765</v>
       </c>
       <c r="Q100" s="65">
@@ -10842,39 +11087,39 @@
         <v>816</v>
       </c>
       <c r="I101" s="65">
-        <f t="shared" ref="I101:Q101" si="123">I4/H4-1</f>
+        <f t="shared" ref="I101:Q101" si="130">I4/H4-1</f>
         <v>-0.11731238792873222</v>
       </c>
       <c r="J101" s="65">
-        <f t="shared" si="123"/>
+        <f t="shared" si="130"/>
         <v>0.61374798070117631</v>
       </c>
       <c r="K101" s="65">
-        <f t="shared" si="123"/>
+        <f t="shared" si="130"/>
         <v>-0.19357387499288559</v>
       </c>
       <c r="L101" s="65">
-        <f t="shared" si="123"/>
+        <f t="shared" si="130"/>
         <v>0.28305012268079333</v>
       </c>
       <c r="M101" s="65">
-        <f t="shared" si="123"/>
+        <f t="shared" si="130"/>
         <v>0.10870191265406226</v>
       </c>
       <c r="N101" s="65">
-        <f t="shared" si="123"/>
+        <f t="shared" si="130"/>
         <v>-3.7715860040100302E-2</v>
       </c>
       <c r="O101" s="65">
-        <f t="shared" si="123"/>
+        <f t="shared" si="130"/>
         <v>-0.14253695582285475</v>
       </c>
       <c r="P101" s="65">
-        <f t="shared" si="123"/>
+        <f t="shared" si="130"/>
         <v>4.9430357136541092E-2</v>
       </c>
       <c r="Q101" s="65">
-        <f t="shared" si="123"/>
+        <f t="shared" si="130"/>
         <v>0.17039326448620784</v>
       </c>
       <c r="R101" s="75"/>
@@ -10885,39 +11130,39 @@
         <v>817</v>
       </c>
       <c r="I102" s="65">
-        <f t="shared" ref="I102:Q102" si="124">I5/H5-1</f>
+        <f t="shared" ref="I102:Q102" si="131">I5/H5-1</f>
         <v>-0.1718722323906241</v>
       </c>
       <c r="J102" s="65">
-        <f t="shared" si="124"/>
+        <f t="shared" si="131"/>
         <v>1.5855553971196352</v>
       </c>
       <c r="K102" s="65">
-        <f t="shared" si="124"/>
+        <f t="shared" si="131"/>
         <v>7.5830690748635021E-4</v>
       </c>
       <c r="L102" s="65">
-        <f t="shared" si="124"/>
+        <f t="shared" si="131"/>
         <v>-0.19132052076875383</v>
       </c>
       <c r="M102" s="65">
-        <f t="shared" si="124"/>
+        <f t="shared" si="131"/>
         <v>-5.019762172476061E-2</v>
       </c>
       <c r="N102" s="65">
-        <f t="shared" si="124"/>
+        <f t="shared" si="131"/>
         <v>0.13310852622799385</v>
       </c>
       <c r="O102" s="65">
-        <f t="shared" si="124"/>
+        <f t="shared" si="131"/>
         <v>-0.15588270212513355</v>
       </c>
       <c r="P102" s="65">
-        <f t="shared" si="124"/>
+        <f t="shared" si="131"/>
         <v>-9.2330051570557958E-2</v>
       </c>
       <c r="Q102" s="65">
-        <f t="shared" si="124"/>
+        <f t="shared" si="131"/>
         <v>2.8924723407341979E-4</v>
       </c>
       <c r="R102" s="75"/>
@@ -10928,39 +11173,39 @@
         <v>819</v>
       </c>
       <c r="I103" s="70">
-        <f t="shared" ref="I103:Q103" si="125">I6/H6-1</f>
+        <f t="shared" ref="I103:Q103" si="132">I6/H6-1</f>
         <v>-0.23828539389738534</v>
       </c>
       <c r="J103" s="70">
-        <f t="shared" si="125"/>
+        <f t="shared" si="132"/>
         <v>1.0549972940599743</v>
       </c>
       <c r="K103" s="70">
-        <f t="shared" si="125"/>
+        <f t="shared" si="132"/>
         <v>-3.8935998856132414E-2</v>
       </c>
       <c r="L103" s="70">
-        <f t="shared" si="125"/>
+        <f t="shared" si="132"/>
         <v>-6.1431667318194938E-2</v>
       </c>
       <c r="M103" s="70">
-        <f t="shared" si="125"/>
+        <f t="shared" si="132"/>
         <v>7.4285635721933918E-2</v>
       </c>
       <c r="N103" s="70">
-        <f t="shared" si="125"/>
+        <f t="shared" si="132"/>
         <v>0.13999233628213337</v>
       </c>
       <c r="O103" s="70">
-        <f t="shared" si="125"/>
+        <f t="shared" si="132"/>
         <v>-1.726150932381687E-2</v>
       </c>
       <c r="P103" s="70">
-        <f t="shared" si="125"/>
+        <f t="shared" si="132"/>
         <v>-0.14652505955360839</v>
       </c>
       <c r="Q103" s="70">
-        <f t="shared" si="125"/>
+        <f t="shared" si="132"/>
         <v>3.3388630685857734E-2</v>
       </c>
       <c r="R103" s="76"/>
@@ -10989,39 +11234,39 @@
         <v>820</v>
       </c>
       <c r="I104" s="65">
-        <f t="shared" ref="I104:Q104" si="126">I7/H7-1</f>
+        <f t="shared" ref="I104:Q104" si="133">I7/H7-1</f>
         <v>-0.68959117130674685</v>
       </c>
       <c r="J104" s="65">
-        <f t="shared" si="126"/>
+        <f t="shared" si="133"/>
         <v>3.0596315449256624</v>
       </c>
       <c r="K104" s="65">
-        <f t="shared" si="126"/>
+        <f t="shared" si="133"/>
         <v>1.170892878468214</v>
       </c>
       <c r="L104" s="65">
-        <f t="shared" si="126"/>
+        <f t="shared" si="133"/>
         <v>-0.60287888511964793</v>
       </c>
       <c r="M104" s="65">
-        <f t="shared" si="126"/>
+        <f t="shared" si="133"/>
         <v>7.4063813085838204E-2</v>
       </c>
       <c r="N104" s="65">
-        <f t="shared" si="126"/>
+        <f t="shared" si="133"/>
         <v>0.33695885817462701</v>
       </c>
       <c r="O104" s="65">
-        <f t="shared" si="126"/>
+        <f t="shared" si="133"/>
         <v>0.17707964886330751</v>
       </c>
       <c r="P104" s="65">
-        <f t="shared" si="126"/>
+        <f t="shared" si="133"/>
         <v>-0.27328853193465552</v>
       </c>
       <c r="Q104" s="65">
-        <f t="shared" si="126"/>
+        <f t="shared" si="133"/>
         <v>5.7627246071723981E-2</v>
       </c>
     </row>
@@ -11030,39 +11275,39 @@
         <v>821</v>
       </c>
       <c r="I105" s="65">
-        <f t="shared" ref="I105:Q105" si="127">I8/H8-1</f>
+        <f t="shared" ref="I105:Q105" si="134">I8/H8-1</f>
         <v>-5.2339367300907602E-3</v>
       </c>
       <c r="J105" s="65">
-        <f t="shared" si="127"/>
+        <f t="shared" si="134"/>
         <v>7.8805848667189871E-2</v>
       </c>
       <c r="K105" s="65">
-        <f t="shared" si="127"/>
+        <f t="shared" si="134"/>
         <v>-0.14270316878637646</v>
       </c>
       <c r="L105" s="65">
-        <f t="shared" si="127"/>
+        <f t="shared" si="134"/>
         <v>-1.0297334674377672</v>
       </c>
       <c r="M105" s="65">
-        <f t="shared" si="127"/>
+        <f t="shared" si="134"/>
         <v>-0.93234672304439747</v>
       </c>
       <c r="N105" s="65">
-        <f t="shared" si="127"/>
+        <f t="shared" si="134"/>
         <v>-3.171875</v>
       </c>
       <c r="O105" s="65">
-        <f t="shared" si="127"/>
+        <f t="shared" si="134"/>
         <v>30.97122302158273</v>
       </c>
       <c r="P105" s="65">
-        <f t="shared" si="127"/>
+        <f t="shared" si="134"/>
         <v>-4.5904590459045824E-2</v>
       </c>
       <c r="Q105" s="65">
-        <f t="shared" si="127"/>
+        <f t="shared" si="134"/>
         <v>0.98396226415094357</v>
       </c>
     </row>
@@ -11075,115 +11320,115 @@
         <v>0.59414882180942552</v>
       </c>
       <c r="I107" s="25">
-        <f t="shared" ref="I107:R107" si="128">I12/I9</f>
+        <f t="shared" ref="I107:R107" si="135">I12/I9</f>
         <v>0.67817816969080325</v>
       </c>
       <c r="J107" s="25">
-        <f t="shared" si="128"/>
+        <f t="shared" si="135"/>
         <v>0.38628115010177799</v>
       </c>
       <c r="K107" s="25">
-        <f t="shared" si="128"/>
+        <f t="shared" si="135"/>
         <v>0.41729034611181637</v>
       </c>
       <c r="L107" s="25">
-        <f t="shared" si="128"/>
+        <f t="shared" si="135"/>
         <v>0.40935415746960502</v>
       </c>
       <c r="M107" s="25">
-        <f t="shared" si="128"/>
+        <f t="shared" si="135"/>
         <v>0.40324771703856505</v>
       </c>
       <c r="N107" s="25">
-        <f t="shared" si="128"/>
+        <f t="shared" si="135"/>
         <v>0.38781726939332217</v>
       </c>
       <c r="O107" s="25">
-        <f t="shared" si="128"/>
+        <f t="shared" si="135"/>
         <v>0.44184134893621202</v>
       </c>
       <c r="P107" s="25">
-        <f t="shared" si="128"/>
+        <f t="shared" si="135"/>
         <v>0.45693399797839268</v>
       </c>
       <c r="Q107" s="25">
-        <f t="shared" si="128"/>
+        <f t="shared" si="135"/>
         <v>0.44157808009594857</v>
       </c>
       <c r="R107" s="72">
-        <f t="shared" si="128"/>
+        <f t="shared" si="135"/>
         <v>0.42895725935022022</v>
       </c>
       <c r="U107" s="25">
-        <f t="shared" ref="U107:AL107" si="129">U12/U9</f>
+        <f t="shared" ref="U107:AL107" si="136">U12/U9</f>
         <v>0.37771430114149451</v>
       </c>
       <c r="V107" s="25">
-        <f t="shared" si="129"/>
+        <f t="shared" si="136"/>
         <v>0.37760351403197812</v>
       </c>
       <c r="W107" s="25">
-        <f t="shared" si="129"/>
+        <f t="shared" si="136"/>
         <v>0.42080964570985102</v>
       </c>
       <c r="X107" s="25">
-        <f t="shared" si="129"/>
+        <f t="shared" si="136"/>
         <v>0.42023132239656397</v>
       </c>
       <c r="Y107" s="25">
-        <f t="shared" si="129"/>
+        <f t="shared" si="136"/>
         <v>0.42409417497036345</v>
       </c>
       <c r="Z107" s="25">
-        <f t="shared" si="129"/>
+        <f t="shared" si="136"/>
         <v>0.48538449900294256</v>
       </c>
       <c r="AA107" s="25">
-        <f t="shared" si="129"/>
+        <f t="shared" si="136"/>
         <v>0.41078648134782536</v>
       </c>
       <c r="AB107" s="72">
-        <f t="shared" si="129"/>
+        <f t="shared" si="136"/>
         <v>0.37352786459200688</v>
       </c>
       <c r="AC107" s="65">
-        <f t="shared" si="129"/>
+        <f t="shared" si="136"/>
         <v>0.3898998698173477</v>
       </c>
       <c r="AD107" s="65">
-        <f t="shared" si="129"/>
+        <f t="shared" si="136"/>
         <v>0.40687889459616033</v>
       </c>
       <c r="AE107" s="65">
-        <f t="shared" si="129"/>
+        <f t="shared" si="136"/>
         <v>0.42449147926761222</v>
       </c>
       <c r="AF107" s="65">
-        <f t="shared" si="129"/>
+        <f t="shared" si="136"/>
         <v>0.44276401542814858</v>
       </c>
       <c r="AG107" s="65">
-        <f t="shared" si="129"/>
+        <f t="shared" si="136"/>
         <v>0.46172244331878237</v>
       </c>
       <c r="AH107" s="65">
-        <f t="shared" si="129"/>
+        <f t="shared" si="136"/>
         <v>0.48172478086605175</v>
       </c>
       <c r="AI107" s="65">
-        <f t="shared" si="129"/>
+        <f t="shared" si="136"/>
         <v>0.48238207549596013</v>
       </c>
       <c r="AJ107" s="65">
-        <f t="shared" si="129"/>
+        <f t="shared" si="136"/>
         <v>0.48294740632301031</v>
       </c>
       <c r="AK107" s="65">
-        <f t="shared" si="129"/>
+        <f t="shared" si="136"/>
         <v>0.48343346744763499</v>
       </c>
       <c r="AL107" s="65">
-        <f t="shared" si="129"/>
+        <f t="shared" si="136"/>
         <v>0.4838512463586328</v>
       </c>
     </row>

</xml_diff>